<commit_message>
improves export of the LCAresults into excel files (shortens names, creates export folder)
</commit_message>
<xml_diff>
--- a/example/inputs/functional_units.xlsx
+++ b/example/inputs/functional_units.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20394"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B776001B-749F-4C7D-B5EB-83FCB22220E7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8E7D99-8AD3-41E2-ADC0-35200038AC85}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
   <si>
     <t>GLO</t>
   </si>
@@ -59,6 +59,27 @@
   </si>
   <si>
     <t>operation only - transport, passenger car, small size, petrol, EURO 5</t>
+  </si>
+  <si>
+    <t>electricity, high voltage</t>
+  </si>
+  <si>
+    <t>treatment of bagasse, from sweet sorghum, in heat and power co-generation unit, 6400kW thermal</t>
+  </si>
+  <si>
+    <t>heat, district or industrial, other than natural gas</t>
+  </si>
+  <si>
+    <t>electricity, low voltage</t>
+  </si>
+  <si>
+    <t>wood pellets, burned in stirling heat and power co-generation unit, 3kW electrical, future</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>heat, future</t>
   </si>
 </sst>
 </file>
@@ -406,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -516,6 +537,62 @@
         <v>9</v>
       </c>
     </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
fixes get_functional_units() and create_calculation_setup()
</commit_message>
<xml_diff>
--- a/example/inputs/functional_units.xlsx
+++ b/example/inputs/functional_units.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC36EC71-9F67-4982-AFE7-6A8668BE7D0D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F6893C-2F74-41C0-AA1F-E79C9E559E1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>GLO</t>
   </si>
@@ -55,12 +55,6 @@
     <t>SS_ei38_remind_Base_RCP19_SETAC2022</t>
   </si>
   <si>
-    <t>operation only - transport, passenger car, electric</t>
-  </si>
-  <si>
-    <t>operation only - transport, passenger car, small size, petrol, EURO 5</t>
-  </si>
-  <si>
     <t>electricity, high voltage</t>
   </si>
   <si>
@@ -79,7 +73,16 @@
     <t>CH</t>
   </si>
   <si>
-    <t>heat, future</t>
+    <t>DE</t>
+  </si>
+  <si>
+    <t>electricity production, natural gas, conventional power plant_OpO_noDC</t>
+  </si>
+  <si>
+    <t>electricity production, nuclear, pressure water reactor_OpO</t>
+  </si>
+  <si>
+    <t>electricity production, natural gas, conventional power plant_4BioG_ConO_OpO_noDC</t>
   </si>
 </sst>
 </file>
@@ -427,15 +430,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="84.7265625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -481,34 +485,6 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
@@ -539,10 +515,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -553,10 +529,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -567,30 +543,58 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
         <v>16</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" t="s">
-        <v>18</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C13" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adds more details to exported excel files for lca results
</commit_message>
<xml_diff>
--- a/example/inputs/functional_units.xlsx
+++ b/example/inputs/functional_units.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20397"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06F6893C-2F74-41C0-AA1F-E79C9E559E1C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CC934A-6A45-40CD-8D3A-FAFAE00190E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
   <si>
     <t>GLO</t>
   </si>
@@ -76,13 +76,22 @@
     <t>DE</t>
   </si>
   <si>
-    <t>electricity production, natural gas, conventional power plant_OpO_noDC</t>
-  </si>
-  <si>
-    <t>electricity production, nuclear, pressure water reactor_OpO</t>
-  </si>
-  <si>
-    <t>electricity production, natural gas, conventional power plant_4BioG_ConO_OpO_noDC</t>
+    <t>prod1</t>
+  </si>
+  <si>
+    <t>prod2</t>
+  </si>
+  <si>
+    <t>prod3</t>
+  </si>
+  <si>
+    <t>act1</t>
+  </si>
+  <si>
+    <t>act2</t>
+  </si>
+  <si>
+    <t>act3</t>
   </si>
 </sst>
 </file>
@@ -433,7 +442,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -485,12 +494,40 @@
         <v>10</v>
       </c>
     </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -501,13 +538,13 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
@@ -515,13 +552,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
@@ -529,35 +566,49 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>9</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>18</v>
@@ -571,7 +622,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="B13" t="s">
         <v>19</v>
@@ -585,7 +636,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>20</v>

</xml_diff>

<commit_message>
updates example with new arg of functional_units_sheet
</commit_message>
<xml_diff>
--- a/example/inputs/functional_units.xlsx
+++ b/example/inputs/functional_units.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1CC934A-6A45-40CD-8D3A-FAFAE00190E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B7233D-F7DE-4567-B7CB-D125BA3CE348}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="FUs" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
@@ -442,7 +442,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
adds comments to example
</commit_message>
<xml_diff>
--- a/example/inputs/functional_units.xlsx
+++ b/example/inputs/functional_units.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20404"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B7233D-F7DE-4567-B7CB-D125BA3CE348}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598D4170-6BBD-4F3F-9BD0-8909C06F8387}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="FUs" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>GLO</t>
   </si>
@@ -46,52 +46,10 @@
     <t>database</t>
   </si>
   <si>
-    <t>eco_export_SS</t>
-  </si>
-  <si>
     <t>ecoinvent38_cutoff</t>
   </si>
   <si>
     <t>SS_ei38_remind_Base_RCP19_SETAC2022</t>
-  </si>
-  <si>
-    <t>electricity, high voltage</t>
-  </si>
-  <si>
-    <t>treatment of bagasse, from sweet sorghum, in heat and power co-generation unit, 6400kW thermal</t>
-  </si>
-  <si>
-    <t>heat, district or industrial, other than natural gas</t>
-  </si>
-  <si>
-    <t>electricity, low voltage</t>
-  </si>
-  <si>
-    <t>wood pellets, burned in stirling heat and power co-generation unit, 3kW electrical, future</t>
-  </si>
-  <si>
-    <t>CH</t>
-  </si>
-  <si>
-    <t>DE</t>
-  </si>
-  <si>
-    <t>prod1</t>
-  </si>
-  <si>
-    <t>prod2</t>
-  </si>
-  <si>
-    <t>prod3</t>
-  </si>
-  <si>
-    <t>act1</t>
-  </si>
-  <si>
-    <t>act2</t>
-  </si>
-  <si>
-    <t>act3</t>
   </si>
 </sst>
 </file>
@@ -439,17 +397,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="43.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="84.7265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="35.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
@@ -477,7 +435,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -491,7 +449,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -505,7 +463,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
@@ -519,132 +477,6 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>